<commit_message>
commit with latest files
</commit_message>
<xml_diff>
--- a/src/test/resources/UserData/DSAlgo.xlsx
+++ b/src/test/resources/UserData/DSAlgo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyajoshi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reshm\eclipse-workspace\GitDSAlgoPortal\DSAlgoPortal\src\test\resources\UserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868CBBDC-56FF-B74B-BF7B-0E48E032B5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19946FAC-BF10-42ED-B2AD-DAEB8779A9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16380" xr2:uid="{131EB914-CC09-6846-A0DC-928CA884D295}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{131EB914-CC09-6846-A0DC-928CA884D295}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Hello098@</t>
   </si>
@@ -51,13 +51,19 @@
   </si>
   <si>
     <t>DSALgo090</t>
+  </si>
+  <si>
+    <t>DSAlgo085</t>
+  </si>
+  <si>
+    <t>Hello@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -71,6 +77,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -80,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -103,15 +117,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -424,18 +453,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912FD05A-0B3B-1F42-9325-D76FED303F4C}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -446,7 +477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -455,7 +486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -464,7 +495,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -473,12 +504,25 @@
       </c>
       <c r="C4" s="1">
         <v>1234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{B345220F-76A2-1843-A126-A4F096529EEB}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{F19DAE32-A2D6-4251-9F02-F4F1DB29F942}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{F25486B7-DB45-4D31-9050-FE69E6D4E5A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>